<commit_message>
More cleanup, more work
</commit_message>
<xml_diff>
--- a/datasets/cluster analysis.xlsx
+++ b/datasets/cluster analysis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="515">
   <si>
     <t>=== Run information ===</t>
   </si>
@@ -1555,6 +1555,21 @@
   <si>
     <t>K-Means</t>
   </si>
+  <si>
+    <t>Kmeans</t>
+  </si>
+  <si>
+    <t>RP</t>
+  </si>
+  <si>
+    <t>PCA</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Random Subset</t>
+  </si>
 </sst>
 </file>
 
@@ -1608,12 +1623,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7564,11 +7579,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="155556480"/>
-        <c:axId val="130924928"/>
+        <c:axId val="122555776"/>
+        <c:axId val="122573952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="155556480"/>
+        <c:axId val="122555776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7577,12 +7592,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130924928"/>
+        <c:crossAx val="122573952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="130924928"/>
+        <c:axId val="122573952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7593,14 +7608,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155556480"/>
+        <c:crossAx val="122555776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12659,11 +12673,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="131504000"/>
-        <c:axId val="131505536"/>
+        <c:axId val="122616064"/>
+        <c:axId val="124133376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="131504000"/>
+        <c:axId val="122616064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12672,12 +12686,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131505536"/>
+        <c:crossAx val="124133376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="131505536"/>
+        <c:axId val="124133376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12688,14 +12702,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131504000"/>
+        <c:crossAx val="122616064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -18642,11 +18655,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="123901824"/>
-        <c:axId val="76238208"/>
+        <c:axId val="125858560"/>
+        <c:axId val="125860096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="123901824"/>
+        <c:axId val="125858560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18655,12 +18668,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76238208"/>
+        <c:crossAx val="125860096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76238208"/>
+        <c:axId val="125860096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18671,14 +18684,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123901824"/>
+        <c:crossAx val="125858560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -23737,11 +23749,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="123550336"/>
-        <c:axId val="107871616"/>
+        <c:axId val="127294848"/>
+        <c:axId val="127304832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="123550336"/>
+        <c:axId val="127294848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23750,12 +23762,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107871616"/>
+        <c:crossAx val="127304832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107871616"/>
+        <c:axId val="127304832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23766,14 +23778,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123550336"/>
+        <c:crossAx val="127294848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -29720,11 +29731,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="127154432"/>
-        <c:axId val="127193856"/>
+        <c:axId val="127385984"/>
+        <c:axId val="127387520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="127154432"/>
+        <c:axId val="127385984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29733,12 +29744,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127193856"/>
+        <c:crossAx val="127387520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="127193856"/>
+        <c:axId val="127387520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29749,7 +29760,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127154432"/>
+        <c:crossAx val="127385984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -34815,11 +34826,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="131480576"/>
-        <c:axId val="131482368"/>
+        <c:axId val="134835584"/>
+        <c:axId val="134845568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="131480576"/>
+        <c:axId val="134835584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -34828,12 +34839,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131482368"/>
+        <c:crossAx val="134845568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="131482368"/>
+        <c:axId val="134845568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -34844,7 +34855,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131480576"/>
+        <c:crossAx val="134835584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -35878,20 +35889,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1904763</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>18847</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>295042</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171252</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="23" name="Picture 22"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -35904,8 +35915,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10677525" y="676275"/>
-          <a:ext cx="1895238" cy="1628572"/>
+          <a:off x="15278100" y="685800"/>
+          <a:ext cx="1866667" cy="1580952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -35916,20 +35927,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1904763</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>180773</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>418867</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171252</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="20" name="Picture 19"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -35942,8 +35953,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10677525" y="1990725"/>
-          <a:ext cx="1895238" cy="1619048"/>
+          <a:off x="13573125" y="685800"/>
+          <a:ext cx="1866667" cy="1580952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -35954,20 +35965,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>9291</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>161725</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>295042</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142673</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="19" name="Picture 18"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -35980,8 +35991,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10715625" y="3324225"/>
-          <a:ext cx="1876191" cy="1600000"/>
+          <a:off x="15278100" y="1952625"/>
+          <a:ext cx="1866667" cy="1619048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -35992,20 +36003,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>18814</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>114098</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>428391</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="18" name="Picture 17"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -36018,8 +36029,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10715625" y="4591050"/>
-          <a:ext cx="1885714" cy="1619048"/>
+          <a:off x="13573125" y="1971675"/>
+          <a:ext cx="1876191" cy="1600000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -36030,20 +36041,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>56914</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>95047</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>295042</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>123625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="17" name="Picture 16"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -36056,8 +36067,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10753725" y="5895975"/>
-          <a:ext cx="1885714" cy="1628572"/>
+          <a:off x="15278100" y="3286125"/>
+          <a:ext cx="1866667" cy="1600000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -36068,20 +36079,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>199788</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>18844</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>456963</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>123625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="16" name="Picture 15"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -36094,160 +36105,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8972550" y="657225"/>
-          <a:ext cx="1895238" cy="1647619"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>190267</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>180774</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8991600" y="2000250"/>
-          <a:ext cx="1866667" cy="1609524"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>247413</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>161723</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9020175" y="3305175"/>
-          <a:ext cx="1895238" cy="1619048"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>237891</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>114102</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9029700" y="4629150"/>
-          <a:ext cx="1876191" cy="1580952"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>247416</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>85527</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9039225" y="5934075"/>
-          <a:ext cx="1876191" cy="1580952"/>
+          <a:off x="13582650" y="3286125"/>
+          <a:ext cx="1895238" cy="1600000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -36282,7 +36141,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -36314,7 +36173,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -36341,7 +36200,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -36379,7 +36238,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -36417,7 +36276,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -36455,7 +36314,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -36493,7 +36352,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -36531,7 +36390,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -36569,7 +36428,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -36607,7 +36466,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -36645,7 +36504,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -36683,7 +36542,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -36692,6 +36551,346 @@
         <a:xfrm>
           <a:off x="8753475" y="17526000"/>
           <a:ext cx="3123810" cy="580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Connector 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8686800" y="1962150"/>
+          <a:ext cx="4314825" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Straight Connector 37"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8639175" y="3267075"/>
+          <a:ext cx="4314825" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Straight Connector 38"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8677275" y="4581525"/>
+          <a:ext cx="4314825" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Straight Connector 39"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8677275" y="5867400"/>
+          <a:ext cx="4314825" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Connector 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9201150" y="495300"/>
+          <a:ext cx="0" cy="6648450"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Straight Connector 40"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10906125" y="466725"/>
+          <a:ext cx="0" cy="6648450"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>295042</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76002</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15278100" y="4591050"/>
+          <a:ext cx="1866667" cy="1580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>409343</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76002</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13573125" y="4591050"/>
+          <a:ext cx="1857143" cy="1580952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -37009,11 +37208,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
         <v>96</v>
@@ -37035,94 +37234,94 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H4" s="5"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H5" s="5"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H6" s="5"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H7" s="5"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H8" s="5"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H9" s="5"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H10" s="6"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H11" s="5"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H12" s="5"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H13" s="5"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H14" s="5"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H15" s="5"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H16" s="5"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H17" s="5"/>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H18" s="5"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H19" s="5"/>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H20" s="5"/>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H21" s="5"/>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H22" s="5"/>
+      <c r="H22" s="4"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H23" s="5"/>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H24" s="5"/>
+      <c r="H24" s="4"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H25" s="5"/>
+      <c r="H25" s="4"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H26" s="5"/>
+      <c r="H26" s="4"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H27" s="5"/>
+      <c r="H27" s="4"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H28" s="5"/>
+      <c r="H28" s="4"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H29" s="5"/>
+      <c r="H29" s="4"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H30" s="5"/>
+      <c r="H30" s="4"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
@@ -37136,40 +37335,40 @@
       <c r="F31" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="H31" s="5"/>
+      <c r="H31" s="4"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H32" s="5"/>
+      <c r="H32" s="4"/>
     </row>
     <row r="33" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H33" s="5"/>
+      <c r="H33" s="4"/>
     </row>
     <row r="34" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H34" s="5"/>
+      <c r="H34" s="4"/>
     </row>
     <row r="35" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H35" s="5"/>
+      <c r="H35" s="4"/>
     </row>
     <row r="36" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H36" s="5"/>
+      <c r="H36" s="4"/>
     </row>
     <row r="37" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H37" s="5"/>
+      <c r="H37" s="4"/>
     </row>
     <row r="38" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H38" s="5"/>
+      <c r="H38" s="4"/>
     </row>
     <row r="39" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H39" s="5"/>
+      <c r="H39" s="4"/>
     </row>
     <row r="40" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H40" s="5"/>
+      <c r="H40" s="4"/>
     </row>
     <row r="41" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H41" s="5"/>
+      <c r="H41" s="4"/>
     </row>
     <row r="42" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H42" s="5"/>
+      <c r="H42" s="4"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="I57" t="s">
@@ -37177,11 +37376,11 @@
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2" t="s">
         <v>96</v>
@@ -37236,8 +37435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L92"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37253,15 +37452,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -37279,94 +37484,106 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H4" s="5"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H5" s="5"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H6" s="5"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H7" s="5"/>
+      <c r="G7" t="s">
+        <v>513</v>
+      </c>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H8" s="5"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H9" s="5"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H10" s="6"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H11" s="5"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H12" s="5"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H13" s="5"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H14" s="5"/>
+      <c r="G14" t="s">
+        <v>512</v>
+      </c>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H15" s="5"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H16" s="5"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H17" s="5"/>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H18" s="5"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H19" s="5"/>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H20" s="5"/>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H21" s="5"/>
+      <c r="G21" t="s">
+        <v>511</v>
+      </c>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H22" s="5"/>
+      <c r="H22" s="4"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H23" s="5"/>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H24" s="5"/>
+      <c r="H24" s="4"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H25" s="5"/>
+      <c r="H25" s="4"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H26" s="5"/>
+      <c r="H26" s="4"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H27" s="5"/>
+      <c r="H27" s="4"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H28" s="5"/>
+      <c r="G28" t="s">
+        <v>514</v>
+      </c>
+      <c r="H28" s="4"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H29" s="5"/>
+      <c r="H29" s="4"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H30" s="5"/>
+      <c r="H30" s="4"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
@@ -37380,40 +37597,40 @@
       <c r="F31" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="H31" s="5"/>
+      <c r="H31" s="4"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H32" s="5"/>
+      <c r="H32" s="4"/>
     </row>
     <row r="33" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H33" s="5"/>
+      <c r="H33" s="4"/>
     </row>
     <row r="34" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H34" s="5"/>
+      <c r="H34" s="4"/>
     </row>
     <row r="35" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H35" s="5"/>
+      <c r="H35" s="4"/>
     </row>
     <row r="36" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H36" s="5"/>
+      <c r="H36" s="4"/>
     </row>
     <row r="37" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H37" s="5"/>
+      <c r="H37" s="4"/>
     </row>
     <row r="38" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H38" s="5"/>
+      <c r="H38" s="4"/>
     </row>
     <row r="39" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H39" s="5"/>
+      <c r="H39" s="4"/>
     </row>
     <row r="40" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H40" s="5"/>
+      <c r="H40" s="4"/>
     </row>
     <row r="41" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H41" s="5"/>
+      <c r="H41" s="4"/>
     </row>
     <row r="42" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H42" s="5"/>
+      <c r="H42" s="4"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="I57" t="s">
@@ -37421,11 +37638,11 @@
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2" t="s">
         <v>96</v>

</xml_diff>